<commit_message>
document changes on git and mapping
</commit_message>
<xml_diff>
--- a/deliverables/documents/mapping.xlsx
+++ b/deliverables/documents/mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="167">
   <si>
     <t>Submission Date</t>
   </si>
@@ -522,9 +522,6 @@
   </si>
   <si>
     <t>will not be used</t>
-  </si>
-  <si>
-    <t>pers_created_at</t>
   </si>
   <si>
     <t>done with created at</t>
@@ -974,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42:I47"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1013,9 +1010,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -2301,9 +2296,6 @@
       <c r="B163" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C163" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="164" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B164" s="10" t="s">
@@ -2318,7 +2310,7 @@
         <v>156</v>
       </c>
       <c r="C165" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="166" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>